<commit_message>
Adm pode visualizar seus dados
</commit_message>
<xml_diff>
--- a/Sprint-4/Sprint_4 Burndown-Backlog.xlsx
+++ b/Sprint-4/Sprint_4 Burndown-Backlog.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Criar Controller cadastro Adm</t>
+  </si>
+  <si>
+    <t>Criar classe Sessao</t>
   </si>
 </sst>
 </file>
@@ -541,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -638,14 +641,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -683,10 +689,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -699,13 +708,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4439,28 +4460,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>15.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.5625</c:v>
+                  <c:v>14.4375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.625</c:v>
+                  <c:v>12.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6875</c:v>
+                  <c:v>10.3125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.75</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.8125</c:v>
+                  <c:v>6.1875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.875</c:v>
+                  <c:v>4.125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9375</c:v>
+                  <c:v>2.0625</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4572,31 +4593,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>15.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.67</c:v>
+                  <c:v>13.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.77</c:v>
+                  <c:v>9.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8299999999999992</c:v>
+                  <c:v>6.8299999999999992</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.879999999999999</c:v>
+                  <c:v>3.879999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.120000000000001</c:v>
+                  <c:v>-2.120000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-7.120000000000001</c:v>
+                  <c:v>-6.120000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-11.120000000000001</c:v>
+                  <c:v>-10.120000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-17.12</c:v>
+                  <c:v>-16.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6761,10 +6782,10 @@
   <sheetPr>
     <tabColor rgb="FF38761D"/>
   </sheetPr>
-  <dimension ref="A1:AB1048537"/>
+  <dimension ref="A1:AB1048538"/>
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6781,16 +6802,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
@@ -6815,27 +6836,27 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35" t="s">
+      <c r="G2" s="37"/>
+      <c r="H2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="37">
         <v>8</v>
       </c>
       <c r="J2" s="3"/>
@@ -6859,9 +6880,9 @@
       <c r="AB2" s="4"/>
     </row>
     <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="30" t="s">
         <v>8</v>
       </c>
@@ -6874,8 +6895,8 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -6897,7 +6918,7 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="58" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -6909,12 +6930,12 @@
       <c r="D4" s="26">
         <v>1</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="38">
         <f>SUM(D4:D6)</f>
         <v>3.5</v>
       </c>
       <c r="F4" s="26"/>
-      <c r="G4" s="39">
+      <c r="G4" s="40">
         <f>SUM(F4:F6)</f>
         <v>0</v>
       </c>
@@ -6941,7 +6962,7 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="25" t="s">
         <v>65</v>
       </c>
@@ -6951,9 +6972,9 @@
       <c r="D5" s="26">
         <v>1</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="26"/>
-      <c r="G5" s="40"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="21" t="s">
         <v>10</v>
       </c>
@@ -6978,7 +6999,7 @@
       <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="6" t="s">
         <v>66</v>
       </c>
@@ -6988,9 +7009,9 @@
       <c r="D6" s="26">
         <v>1.5</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="26"/>
-      <c r="G6" s="40"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="21" t="s">
         <v>10</v>
       </c>
@@ -7013,116 +7034,132 @@
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
     </row>
-    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
-        <v>71</v>
-      </c>
+    <row r="7" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="60"/>
       <c r="B7" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="28">
-        <v>3</v>
-      </c>
-      <c r="E7" s="34">
-        <f>SUM(D7:D9)</f>
-        <v>7.5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E7" s="61"/>
       <c r="F7" s="28"/>
-      <c r="G7" s="34">
-        <f>SUM(F7:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>10</v>
-      </c>
+      <c r="G7" s="62"/>
+      <c r="H7" s="21"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="B8" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="34"/>
+        <v>3</v>
+      </c>
+      <c r="E8" s="36">
+        <f>SUM(D8:D10)</f>
+        <v>7.5</v>
+      </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="34"/>
+      <c r="G8" s="36">
+        <f>SUM(F8:F10)</f>
+        <v>0</v>
+      </c>
       <c r="H8" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
-      <c r="B9" s="33" t="s">
-        <v>69</v>
+    <row r="9" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="35"/>
+      <c r="B9" s="29" t="s">
+        <v>68</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="28">
-        <v>4</v>
-      </c>
-      <c r="E9" s="34"/>
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="36"/>
       <c r="F9" s="28"/>
-      <c r="G9" s="34"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>73</v>
+    <row r="10" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="35"/>
+      <c r="B10" s="33" t="s">
+        <v>69</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="34">
-        <f>SUM(D10:D12)</f>
-        <v>4.5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E10" s="36"/>
       <c r="F10" s="28"/>
-      <c r="G10" s="34">
-        <f>SUM(F10:F12)</f>
-        <v>0</v>
-      </c>
+      <c r="G10" s="36"/>
       <c r="H10" s="21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
+      <c r="A11" s="35" t="s">
+        <v>72</v>
+      </c>
       <c r="B11" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="28">
-        <v>2</v>
-      </c>
-      <c r="E11" s="34"/>
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="36">
+        <f>SUM(D11:D13)</f>
+        <v>4.5</v>
+      </c>
       <c r="F11" s="28"/>
-      <c r="G11" s="34"/>
+      <c r="G11" s="36">
+        <f>SUM(F11:F13)</f>
+        <v>0</v>
+      </c>
       <c r="H11" s="21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
-      <c r="B12" s="33" t="s">
-        <v>74</v>
+      <c r="A12" s="35"/>
+      <c r="B12" s="29" t="s">
+        <v>75</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>25</v>
@@ -7130,25 +7167,38 @@
       <c r="D12" s="28">
         <v>2</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="28"/>
-      <c r="G12" s="34"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="1048533" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" s="35"/>
+      <c r="B13" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="28">
+        <v>2</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="1048534" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048535" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048536" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048537" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048538" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="I2:I3"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -7156,11 +7206,16 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="G4:G7"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I3">
     <cfRule type="expression" dxfId="252" priority="2">
@@ -7173,7 +7228,7 @@
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="E7 G7 E4" formulaRange="1"/>
+    <ignoredError sqref="E8 G8 E4" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -7208,20 +7263,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42" t="s">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
@@ -7280,40 +7335,40 @@
       <c r="S2" s="8"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43">
+      <c r="A3" s="44">
         <v>8</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="45" t="s">
         <v>17</v>
       </c>
       <c r="M3" s="8"/>
@@ -7325,18 +7380,18 @@
       <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
@@ -7351,35 +7406,35 @@
       </c>
       <c r="B5" s="13">
         <f>SUM('Sprint Backlog'!D:D)</f>
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="C5" s="14">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>13.5625</v>
+        <v>14.4375</v>
       </c>
       <c r="D5" s="14">
         <f t="shared" si="1"/>
-        <v>11.625</v>
+        <v>12.375</v>
       </c>
       <c r="E5" s="14">
         <f t="shared" si="1"/>
-        <v>9.6875</v>
+        <v>10.3125</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="1"/>
-        <v>7.75</v>
+        <v>8.25</v>
       </c>
       <c r="G5" s="14">
         <f t="shared" si="1"/>
-        <v>5.8125</v>
+        <v>6.1875</v>
       </c>
       <c r="H5" s="14">
         <f t="shared" si="1"/>
-        <v>3.875</v>
+        <v>4.125</v>
       </c>
       <c r="I5" s="14">
         <f t="shared" si="1"/>
-        <v>1.9375</v>
+        <v>2.0625</v>
       </c>
       <c r="J5" s="14">
         <f t="shared" si="1"/>
@@ -7387,11 +7442,11 @@
       </c>
       <c r="K5" s="14">
         <f>SUM(C5:J5)</f>
-        <v>54.25</v>
+        <v>57.75</v>
       </c>
       <c r="L5" s="14">
         <f>K5/A$3</f>
-        <v>6.78125</v>
+        <v>7.21875</v>
       </c>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -7407,47 +7462,47 @@
       </c>
       <c r="B6" s="13">
         <f>B5</f>
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="C6" s="14">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>12.67</v>
+        <v>13.67</v>
       </c>
       <c r="D6" s="14">
         <f t="shared" si="2"/>
-        <v>8.77</v>
+        <v>9.77</v>
       </c>
       <c r="E6" s="14">
         <f t="shared" si="2"/>
-        <v>5.8299999999999992</v>
+        <v>6.8299999999999992</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="2"/>
-        <v>2.879999999999999</v>
+        <v>3.879999999999999</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" si="2"/>
-        <v>-3.120000000000001</v>
+        <v>-2.120000000000001</v>
       </c>
       <c r="H6" s="14">
         <f t="shared" si="2"/>
-        <v>-7.120000000000001</v>
+        <v>-6.120000000000001</v>
       </c>
       <c r="I6" s="14">
         <f t="shared" si="2"/>
-        <v>-11.120000000000001</v>
+        <v>-10.120000000000001</v>
       </c>
       <c r="J6" s="14">
         <f t="shared" si="2"/>
-        <v>-17.12</v>
+        <v>-16.12</v>
       </c>
       <c r="K6" s="14">
         <f>SUM(C6:J6)</f>
-        <v>-8.330000000000009</v>
+        <v>-0.33000000000001606</v>
       </c>
       <c r="L6" s="14">
         <f>K6/A$3</f>
-        <v>-1.0412500000000011</v>
+        <v>-4.1250000000002007E-2</v>
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -7485,18 +7540,18 @@
       <c r="B8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -7511,7 +7566,7 @@
       </c>
       <c r="B9" s="17">
         <f>B5/A3</f>
-        <v>1.9375</v>
+        <v>2.0625</v>
       </c>
       <c r="C9" s="17">
         <f t="shared" ref="C9:K9" si="3">SUM(C10:C12)</f>
@@ -8796,20 +8851,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42" t="s">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
@@ -8868,40 +8923,40 @@
       <c r="S2" s="8"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43">
+      <c r="A3" s="44">
         <v>8</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="45" t="s">
         <v>17</v>
       </c>
       <c r="M3" s="8"/>
@@ -8913,18 +8968,18 @@
       <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
@@ -9072,18 +9127,18 @@
       <c r="B8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -9149,10 +9204,10 @@
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="52"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="14">
         <v>0.75</v>
       </c>
@@ -9172,18 +9227,18 @@
         <v>9.375E-2</v>
       </c>
       <c r="M10" s="8"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="50"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="48"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="14">
         <v>0.83</v>
       </c>
@@ -9211,10 +9266,10 @@
       <c r="S11" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="48"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14">
@@ -9242,10 +9297,10 @@
       <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="48"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="14">
         <v>1.25</v>
       </c>
@@ -9265,18 +9320,18 @@
         <v>0.15625</v>
       </c>
       <c r="M13" s="8"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="49"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="48"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14">
@@ -9304,10 +9359,10 @@
       <c r="S14" s="8"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="48"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14">
@@ -9327,18 +9382,18 @@
         <v>0.19875000000000001</v>
       </c>
       <c r="M15" s="8"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="49"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14">
         <v>3.4</v>
@@ -9358,18 +9413,18 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="M16" s="8"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="52"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="52"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -9390,10 +9445,10 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="48"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -9414,10 +9469,10 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="48"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
@@ -9438,10 +9493,10 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="54"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -9462,10 +9517,10 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="48"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -9486,10 +9541,10 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="48"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
@@ -9510,10 +9565,10 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="56"/>
+      <c r="B23" s="51"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -9534,12 +9589,12 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="47"/>
-      <c r="B24" s="48"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="49"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="55"/>
-      <c r="B25" s="56"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="51"/>
     </row>
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9547,17 +9602,18 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A3:A4"/>
@@ -9570,18 +9626,17 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:L10 C24:L96 C19:L21 A19:B19 C13:L13 C15:L16">
     <cfRule type="expression" dxfId="47" priority="37">
@@ -9773,20 +9828,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42" t="s">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
@@ -9845,40 +9900,40 @@
       <c r="S2" s="8"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43">
+      <c r="A3" s="44">
         <v>8</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="45" t="s">
         <v>17</v>
       </c>
       <c r="M3" s="8"/>
@@ -9890,18 +9945,18 @@
       <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
@@ -10049,18 +10104,18 @@
       <c r="B8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -10126,10 +10181,10 @@
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -10157,10 +10212,10 @@
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="48"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14">
         <v>0.5</v>
@@ -10188,10 +10243,10 @@
       <c r="S11" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="48"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14">
@@ -10219,10 +10274,10 @@
       <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="56"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -10250,10 +10305,10 @@
       <c r="S13" s="8"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="54"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="23"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -10274,10 +10329,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="48"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -10298,10 +10353,10 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -10322,10 +10377,10 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -10351,6 +10406,15 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A3:A4"/>
@@ -10365,15 +10429,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="A10:L13 A18:L94">
     <cfRule type="expression" dxfId="12" priority="10">
@@ -10440,20 +10495,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42" t="s">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
@@ -10512,40 +10567,40 @@
       <c r="S2" s="8"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43">
+      <c r="A3" s="44">
         <v>8</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="45" t="s">
         <v>17</v>
       </c>
       <c r="M3" s="8"/>
@@ -10557,18 +10612,18 @@
       <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
@@ -10717,18 +10772,18 @@
       <c r="B8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -10794,8 +10849,8 @@
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="54"/>
-      <c r="B10" s="54"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -10821,8 +10876,8 @@
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="56"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -10848,8 +10903,8 @@
       <c r="S11" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="49"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -10875,8 +10930,8 @@
       <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="54"/>
-      <c r="B13" s="54"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -10907,6 +10962,11 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A3:A4"/>
@@ -10921,11 +10981,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:L96">
     <cfRule type="expression" dxfId="4" priority="2">

</xml_diff>